<commit_message>
Adapted for validation (mail addresses) and sim score api implementation
</commit_message>
<xml_diff>
--- a/lp-ontology-recommender/src/main/resources/testdata/kpi/IndividualsPerformanceKPIs_20160630.xlsx
+++ b/lp-ontology-recommender/src/main/resources/testdata/kpi/IndividualsPerformanceKPIs_20160630.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="45" windowWidth="15000" windowHeight="6990" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="45" windowWidth="15000" windowHeight="6990" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Barnaby Barnes" sheetId="1" r:id="rId1"/>
@@ -120,10 +120,10 @@
   }</t>
   </si>
   <si>
-    <t>barnaby.barnes@learnpad.eu</t>
-  </si>
-  <si>
-    <t>sally.shugar@learnpad.eu</t>
+    <t>b.barnes@learnpad.eu</t>
+  </si>
+  <si>
+    <t>s.shugar@learnpad.eu</t>
   </si>
 </sst>
 </file>
@@ -639,8 +639,8 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A2:E12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,7 +834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -921,7 +921,7 @@
       </c>
       <c r="C5" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>barnaby.barnes@learnpad.eu</v>
+        <v>b.barnes@learnpad.eu</v>
       </c>
       <c r="D5" s="7">
         <f t="shared" ca="1" si="0"/>
@@ -950,7 +950,7 @@
       </c>
       <c r="C6" s="7" t="str">
         <f t="shared" ca="1" si="0"/>
-        <v>sally.shugar@learnpad.eu</v>
+        <v>s.shugar@learnpad.eu</v>
       </c>
       <c r="D6" s="7">
         <f t="shared" ca="1" si="0"/>

</xml_diff>